<commit_message>
Found a partial solution that hit SEQUENCE run length
</commit_message>
<xml_diff>
--- a/Excel_Challenge_508 - Number is Perfect Square and Sum of Squares of Digits is also a Perfect Square.xlsx
+++ b/Excel_Challenge_508 - Number is Perfect Square and Sum of Squares of Digits is also a Perfect Square.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EF9F78-751A-4522-9351-50E440A5E6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C017391-3A29-4021-88CE-A490D417C73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -566,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3087,4 +3110,2661 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34D53AD-D1D9-449B-ADBF-99E3A90ED89B}">
+  <dimension ref="A1:K501"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2:D42">_xlfn.LET(
+_xlpm.fx, _xlfn.LAMBDA(_xlpm.x,SUM(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1)^2)),
+_xlpm.gx, _xlfn.LAMBDA(_xlpm.x,INT(_xlpm.x)=_xlpm.x),
+_xlpm.x,_xlfn.SEQUENCE(1000000,1,100,1),
+_xlpm.z, _xlfn.REDUCE("",_xlpm.x,
+       _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+              IF(AND(_xlpm.gx(_xlpm.v^0.5),_xlpm.gx(_xlpm.fx(_xlpm.v)^0.5)),_xlfn.VSTACK(_xlpm.a,_xlpm.v),_xlpm.a))),
+_xlfn.DROP(_xlpm.z,1))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>400</v>
+      </c>
+      <c r="D3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>676</v>
+      </c>
+      <c r="D4">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>841</v>
+      </c>
+      <c r="D5">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>900</v>
+      </c>
+      <c r="D6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1444</v>
+      </c>
+      <c r="D7">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4225</v>
+      </c>
+      <c r="D8">
+        <v>4225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10000</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>24025</v>
+      </c>
+      <c r="D10">
+        <v>24025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>40000</v>
+      </c>
+      <c r="D11">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>42025</v>
+      </c>
+      <c r="D12">
+        <v>42025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>42436</v>
+      </c>
+      <c r="D13">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>43264</v>
+      </c>
+      <c r="D14">
+        <v>43264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>66049</v>
+      </c>
+      <c r="D15">
+        <v>66049</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>67600</v>
+      </c>
+      <c r="D16">
+        <v>67600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>84100</v>
+      </c>
+      <c r="D17">
+        <v>84100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>90000</v>
+      </c>
+      <c r="D18">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>109561</v>
+      </c>
+      <c r="D19">
+        <v>109561</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>119716</v>
+      </c>
+      <c r="D20">
+        <v>119716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>144400</v>
+      </c>
+      <c r="D21">
+        <v>144400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>155236</v>
+      </c>
+      <c r="D22">
+        <v>155236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>239121</v>
+      </c>
+      <c r="D23">
+        <v>239121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>244036</v>
+      </c>
+      <c r="D24">
+        <v>244036</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>248004</v>
+      </c>
+      <c r="D25">
+        <v>248004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>252004</v>
+      </c>
+      <c r="D26">
+        <v>252004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>335241</v>
+      </c>
+      <c r="D27">
+        <v>335241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>355216</v>
+      </c>
+      <c r="D28">
+        <v>355216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>362404</v>
+      </c>
+      <c r="D29">
+        <v>362404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>373321</v>
+      </c>
+      <c r="D30">
+        <v>373321</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>422500</v>
+      </c>
+      <c r="D31">
+        <v>422500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>643204</v>
+      </c>
+      <c r="D32">
+        <v>643204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>664225</v>
+      </c>
+      <c r="D33">
+        <v>664225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>703921</v>
+      </c>
+      <c r="D34">
+        <v>703921</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>717409</v>
+      </c>
+      <c r="D35">
+        <v>717409</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>751689</v>
+      </c>
+      <c r="D36">
+        <v>751689</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>790321</v>
+      </c>
+      <c r="D37">
+        <v>790321</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>802816</v>
+      </c>
+      <c r="D38">
+        <v>802816</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>840889</v>
+      </c>
+      <c r="D39">
+        <v>840889</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>850084</v>
+      </c>
+      <c r="D40">
+        <v>850084</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>851929</v>
+      </c>
+      <c r="D41">
+        <v>851929</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1000000</v>
+      </c>
+      <c r="D42">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1110916</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1263376</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1292769</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1334025</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1361889</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1366561</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1371241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1413721</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1522756</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1718721</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1750329</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1907161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1951609</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2169729</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2175625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2217121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2226064</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2402500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2640625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2663424</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2765569</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2913849</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>3020644</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>3055504</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>3150625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>3305124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>3374569</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>3381921</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>3545689</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>3587236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>3602404</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>3740356</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>3771364</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>3845521</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>3865156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>4020025</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>4024036</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>4032064</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>4157521</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>4202500</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>4243600</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>4326400</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>4734976</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>5053504</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>5103081</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>5433561</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>5550736</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>5583769</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>5645376</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>5924356</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>5992704</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>6061444</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>6175225</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>6517809</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>6604900</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>6760000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>6848689</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>7054336</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>7273809</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>7974976</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>8059921</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>8311689</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>8375236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>8410000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>8590761</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>8868484</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>8988004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>9162729</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>9217296</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>9511056</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>9765625</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>9891025</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>9979281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>10023556</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>10150596</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>10259209</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>10530025</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>10569001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>10640644</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>10725625</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>10956100</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>11148921</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>11276164</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>11417641</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>11451456</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>11485321</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>11703241</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>11971600</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>12075625</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>12138256</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>12215025</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>12418576</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>12567025</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>12752041</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>12823561</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>12938409</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>13089924</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>13147876</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>13329801</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>13816089</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>13845841</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>14167696</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>14182756</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>14258176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>14341369</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>14440000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>14753281</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>15100996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>15116544</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>15163236</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>15327225</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>15374241</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>15507844</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>15523600</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>15768841</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>15776784</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>15784729</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>16434916</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>16711744</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>16859236</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>16933225</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>17073424</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>17405584</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>17447329</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>17505856</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>17522596</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>18361225</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>18567481</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>19368801</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>19501056</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>19545241</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>20115225</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>20448484</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>20866624</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>21325924</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>21511044</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>21566736</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>21576025</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>21930489</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>21977344</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>22591009</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>22619536</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>22934521</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>23011209</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>23503104</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>23561316</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>23580736</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>23677956</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>23736384</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>23833924</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>23912100</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>23951236</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>24000201</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>24226084</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>24403600</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>24482704</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>24571849</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>24800400</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>25020004</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>25200400</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>25361296</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>25593481</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>25715041</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>26020201</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>26030404</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>26553409</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>26563716</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>26604964</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>26635921</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>26759929</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>27060804</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>27520516</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>27531009</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>27594009</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>27615025</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>27899524</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>27952369</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>28026436</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>28334329</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>28451556</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>29127609</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>29235649</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>29571844</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>29637136</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>30008484</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>30217009</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>30316036</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>30713764</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>31158724</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>31304025</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>31629376</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>32171584</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>32307856</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>32752729</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>33396841</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>33524100</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>33732864</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>34774609</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>35034561</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>35058241</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>35295481</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>35521600</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>35628961</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>35676729</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>35748441</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>36024004</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>36156169</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>36192256</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>36240400</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>36372961</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>36505764</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>36820624</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>37027225</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>37332100</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>38056561</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>38551681</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>39200121</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>39463524</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>39639616</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>39891856</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>40335201</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>41242084</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>41434969</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>41499364</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>41538025</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>42250000</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>43256929</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>43414921</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>43718544</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>43758225</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>44169316</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>44275716</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>44395569</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>45792289</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>45914176</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>46335249</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>46703556</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>46826649</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>47141956</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>47430769</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>48525156</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>48888064</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>49350625</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>49434961</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>49857721</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>50495236</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>50637456</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>50879689</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>51051025</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>51652969</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>51782416</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>52215076</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>53085796</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>53158681</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>53231616</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>53494596</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>53714241</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>53758224</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>54390625</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>54479161</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>55071241</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>55547209</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>55771024</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>55845729</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>56235001</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>57229225</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>58155876</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>58232161</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>58614336</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>58813561</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>59043856</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>59521225</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>60233121</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>60637369</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>60777616</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>61121124</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>61136761</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>62031376</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>62837329</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>63313849</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>63345681</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>63536841</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>64032004</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>64176121</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>64320400</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>64899136</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>65237929</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>65755881</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>66113161</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>66373609</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>66422500</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>66732561</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>69655716</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>69705801</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>69973225</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>70392100</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>70711281</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>70997476</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>71740900</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>72029169</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>72165025</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347">
+        <v>72301009</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348">
+        <v>73034116</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349">
+        <v>73051209</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350">
+        <v>73136704</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351">
+        <v>73702225</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352">
+        <v>74425129</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353">
+        <v>74787904</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354">
+        <v>74909025</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355">
+        <v>75168900</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356">
+        <v>75186241</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357">
+        <v>75481344</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358">
+        <v>75498721</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359">
+        <v>75986089</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360">
+        <v>76143076</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361">
+        <v>76195441</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362">
+        <v>76230361</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363">
+        <v>76632516</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364">
+        <v>76983076</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365">
+        <v>77457601</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366">
+        <v>77704225</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367">
+        <v>78039556</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368">
+        <v>78712384</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369">
+        <v>79032100</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370">
+        <v>79584241</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371">
+        <v>80048809</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372">
+        <v>80281600</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373">
+        <v>81631225</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374">
+        <v>81757764</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A375">
+        <v>82228624</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376">
+        <v>82591744</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377">
+        <v>82646281</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378">
+        <v>84088900</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379">
+        <v>84879369</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380">
+        <v>84971524</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381">
+        <v>85008400</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382">
+        <v>85192900</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383">
+        <v>85877289</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384">
+        <v>86155524</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385">
+        <v>86266944</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386">
+        <v>86452804</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387">
+        <v>86806489</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A388">
+        <v>87815641</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389">
+        <v>88717561</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A390">
+        <v>89889361</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391">
+        <v>91661476</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392">
+        <v>92217609</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393">
+        <v>93412225</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394">
+        <v>93818596</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395">
+        <v>94109401</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396">
+        <v>94167616</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397">
+        <v>94497841</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398">
+        <v>94517284</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399">
+        <v>94945536</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400">
+        <v>95394289</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401">
+        <v>95922436</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A402">
+        <v>96255721</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A403">
+        <v>96550276</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A404">
+        <v>97772544</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A405">
+        <v>98109025</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A406">
+        <v>99102025</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A407">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A408">
+        <v>100881936</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A409">
+        <v>101425041</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A410">
+        <v>102171664</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A411">
+        <v>102232321</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A412">
+        <v>102515625</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A413">
+        <v>103164649</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A414">
+        <v>103286569</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A415">
+        <v>103449241</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A416">
+        <v>105083001</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A417">
+        <v>105144516</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A418">
+        <v>106172416</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A419">
+        <v>106275481</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A420">
+        <v>107143201</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A421">
+        <v>107785924</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A422">
+        <v>108826624</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A423">
+        <v>109098025</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A424">
+        <v>109307025</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A425">
+        <v>109474369</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A426">
+        <v>109725625</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A427">
+        <v>110502144</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A428">
+        <v>110565225</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A429">
+        <v>110796676</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A430">
+        <v>111091600</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A431">
+        <v>111746041</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A432">
+        <v>113678244</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A433">
+        <v>114169225</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A434">
+        <v>114233344</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A435">
+        <v>114340249</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A436">
+        <v>114554209</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A437">
+        <v>115025625</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A438">
+        <v>115863696</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A439">
+        <v>115949824</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A440">
+        <v>116445681</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A441">
+        <v>116748025</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A442">
+        <v>117440569</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A443">
+        <v>117548964</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A444">
+        <v>118265625</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A445">
+        <v>118461456</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446">
+        <v>118657449</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447">
+        <v>119224561</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448">
+        <v>120582361</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449">
+        <v>121176064</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A450">
+        <v>121242121</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A451">
+        <v>121550625</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A452">
+        <v>121638841</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A453">
+        <v>121705024</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A454">
+        <v>122014116</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A455">
+        <v>122301481</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A456">
+        <v>122389969</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A457">
+        <v>122899396</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A458">
+        <v>122943744</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A459">
+        <v>123232201</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A460">
+        <v>123988225</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A461">
+        <v>124925329</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A462">
+        <v>125686521</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A463">
+        <v>125708944</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A464">
+        <v>126337600</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A465">
+        <v>127035441</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A466">
+        <v>127057984</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A467">
+        <v>127893481</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A468">
+        <v>128323584</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A469">
+        <v>128527569</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A470">
+        <v>128754409</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A471">
+        <v>129254161</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A472">
+        <v>129276900</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A473">
+        <v>132089049</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A474">
+        <v>132388036</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A475">
+        <v>132457081</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A476">
+        <v>133402500</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A477">
+        <v>133726096</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A478">
+        <v>134003776</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A479">
+        <v>134722449</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A480">
+        <v>136188900</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A481">
+        <v>136328976</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A482">
+        <v>136656100</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A483">
+        <v>137124100</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A484">
+        <v>137663289</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A485">
+        <v>141348321</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A486">
+        <v>141372100</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A487">
+        <v>142348761</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A488">
+        <v>143209089</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A489">
+        <v>143856036</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A490">
+        <v>143928009</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A491">
+        <v>145274809</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A492">
+        <v>145805625</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A493">
+        <v>147501025</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A494">
+        <v>147671104</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A495">
+        <v>147889921</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A496">
+        <v>148011556</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A497">
+        <v>148035889</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A498">
+        <v>148133241</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A499">
+        <v>149132944</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A500">
+        <v>149377284</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A501">
+        <v>150038001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Found a complete solution using a workaround for the SEQUENCE limitation. I need to understand this limitation better.
</commit_message>
<xml_diff>
--- a/Excel_Challenge_508 - Number is Perfect Square and Sum of Squares of Digits is also a Perfect Square.xlsx
+++ b/Excel_Challenge_508 - Number is Perfect Square and Sum of Squares of Digits is also a Perfect Square.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C017391-3A29-4021-88CE-A490D417C73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AD438E-F2BC-48D9-AD3C-DE87C95EA86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3116,13 +3116,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34D53AD-D1D9-449B-ADBF-99E3A90ED89B}">
   <dimension ref="A1:K501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A496" workbookViewId="0">
+      <selection activeCell="H498" sqref="H498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -3138,10 +3139,10 @@
         <v>100</v>
       </c>
       <c r="D2" cm="1">
-        <f t="array" ref="D2:D42">_xlfn.LET(
+        <f t="array" ref="D2:D501">_xlfn.LET(
 _xlpm.fx, _xlfn.LAMBDA(_xlpm.x,SUM(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1)^2)),
 _xlpm.gx, _xlfn.LAMBDA(_xlpm.x,INT(_xlpm.x)=_xlpm.x),
-_xlpm.x,_xlfn.SEQUENCE(1000000,1,100,1),
+_xlpm.x,_xlfn.SEQUENCE(12250,,4)^2,
 _xlpm.z, _xlfn.REDUCE("",_xlpm.x,
        _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
               IF(AND(_xlpm.gx(_xlpm.v^0.5),_xlpm.gx(_xlpm.fx(_xlpm.v)^0.5)),_xlfn.VSTACK(_xlpm.a,_xlpm.v),_xlpm.a))),
@@ -3473,2294 +3474,3671 @@
       <c r="A43">
         <v>1110916</v>
       </c>
+      <c r="D43">
+        <v>1110916</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1263376</v>
       </c>
+      <c r="D44">
+        <v>1263376</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1292769</v>
       </c>
+      <c r="D45">
+        <v>1292769</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1334025</v>
       </c>
+      <c r="D46">
+        <v>1334025</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1361889</v>
       </c>
+      <c r="D47">
+        <v>1361889</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1366561</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>1366561</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1371241</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>1371241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1413721</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>1413721</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1522756</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>1522756</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1718721</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>1718721</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1750329</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>1750329</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1907161</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>1907161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1951609</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>1951609</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2169729</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>2169729</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2175625</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>2175625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2217121</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>2217121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2226064</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>2226064</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2402500</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>2402500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2640625</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>2640625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2663424</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>2663424</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2765569</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>2765569</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2913849</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>2913849</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3020644</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>3020644</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3055504</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>3055504</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3150625</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>3150625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3305124</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>3305124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3374569</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>3374569</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3381921</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>3381921</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3545689</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>3545689</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3587236</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>3587236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3602404</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>3602404</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3740356</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>3740356</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>3771364</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>3771364</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3845521</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>3845521</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>3865156</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>3865156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4020025</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>4020025</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4024036</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>4024036</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4032064</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>4032064</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4157521</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>4157521</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4202500</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>4202500</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4243600</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>4243600</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4326400</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>4326400</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4734976</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>4734976</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>5053504</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>5053504</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>5103081</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>5103081</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>5433561</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>5433561</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>5550736</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>5550736</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>5583769</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>5583769</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>5645376</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>5645376</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>5924356</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>5924356</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>5992704</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>5992704</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>6061444</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>6061444</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>6175225</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>6175225</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>6517809</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>6517809</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>6604900</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>6604900</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>6760000</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>6760000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>6848689</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>6848689</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>7054336</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>7054336</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>7273809</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>7273809</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>7974976</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>7974976</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>8059921</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>8059921</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>8311689</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>8311689</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>8375236</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>8375236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>8410000</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>8410000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>8590761</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>8590761</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>8868484</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>8868484</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>8988004</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>8988004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>9000000</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>9162729</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>9162729</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>9217296</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>9217296</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>9511056</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>9511056</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>9765625</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>9765625</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>9891025</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>9891025</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>9979281</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>9979281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>10023556</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <v>10023556</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>10150596</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D119">
+        <v>10150596</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>10259209</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D120">
+        <v>10259209</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>10530025</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D121">
+        <v>10530025</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>10569001</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D122">
+        <v>10569001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>10640644</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <v>10640644</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>10725625</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D124">
+        <v>10725625</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>10956100</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D125">
+        <v>10956100</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>11148921</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D126">
+        <v>11148921</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>11276164</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D127">
+        <v>11276164</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>11417641</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D128">
+        <v>11417641</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>11451456</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D129">
+        <v>11451456</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>11485321</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D130">
+        <v>11485321</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>11703241</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D131">
+        <v>11703241</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>11971600</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D132">
+        <v>11971600</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>12075625</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D133">
+        <v>12075625</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>12138256</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D134">
+        <v>12138256</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>12215025</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D135">
+        <v>12215025</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>12418576</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D136">
+        <v>12418576</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>12567025</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D137">
+        <v>12567025</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>12752041</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D138">
+        <v>12752041</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>12823561</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D139">
+        <v>12823561</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>12938409</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D140">
+        <v>12938409</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>13089924</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D141">
+        <v>13089924</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>13147876</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D142">
+        <v>13147876</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>13329801</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D143">
+        <v>13329801</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>13816089</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D144">
+        <v>13816089</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>13845841</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D145">
+        <v>13845841</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>14167696</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D146">
+        <v>14167696</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>14182756</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D147">
+        <v>14182756</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>14258176</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D148">
+        <v>14258176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>14341369</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D149">
+        <v>14341369</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>14440000</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D150">
+        <v>14440000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>14753281</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D151">
+        <v>14753281</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>15100996</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D152">
+        <v>15100996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>15116544</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D153">
+        <v>15116544</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>15163236</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D154">
+        <v>15163236</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>15327225</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D155">
+        <v>15327225</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>15374241</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D156">
+        <v>15374241</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>15507844</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D157">
+        <v>15507844</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>15523600</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D158">
+        <v>15523600</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>15768841</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D159">
+        <v>15768841</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>15776784</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D160">
+        <v>15776784</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>15784729</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D161">
+        <v>15784729</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>16434916</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D162">
+        <v>16434916</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>16711744</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D163">
+        <v>16711744</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>16777216</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D164">
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>16859236</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D165">
+        <v>16859236</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>16933225</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D166">
+        <v>16933225</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>17073424</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D167">
+        <v>17073424</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>17405584</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D168">
+        <v>17405584</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>17447329</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D169">
+        <v>17447329</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>17505856</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D170">
+        <v>17505856</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>17522596</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D171">
+        <v>17522596</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>18361225</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D172">
+        <v>18361225</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>18567481</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D173">
+        <v>18567481</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>19368801</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D174">
+        <v>19368801</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>19501056</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D175">
+        <v>19501056</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>19545241</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D176">
+        <v>19545241</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>20115225</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D177">
+        <v>20115225</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>20448484</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D178">
+        <v>20448484</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>20866624</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D179">
+        <v>20866624</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>21325924</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D180">
+        <v>21325924</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>21511044</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D181">
+        <v>21511044</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>21566736</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D182">
+        <v>21566736</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>21576025</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D183">
+        <v>21576025</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>21930489</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D184">
+        <v>21930489</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>21977344</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D185">
+        <v>21977344</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>22591009</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D186">
+        <v>22591009</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>22619536</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D187">
+        <v>22619536</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>22934521</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D188">
+        <v>22934521</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>23011209</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D189">
+        <v>23011209</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>23503104</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D190">
+        <v>23503104</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>23561316</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D191">
+        <v>23561316</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>23580736</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D192">
+        <v>23580736</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>23677956</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D193">
+        <v>23677956</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>23736384</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D194">
+        <v>23736384</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>23833924</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D195">
+        <v>23833924</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>23912100</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D196">
+        <v>23912100</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>23951236</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D197">
+        <v>23951236</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>24000201</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D198">
+        <v>24000201</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>24226084</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D199">
+        <v>24226084</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>24403600</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D200">
+        <v>24403600</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>24482704</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D201">
+        <v>24482704</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>24571849</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D202">
+        <v>24571849</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>24800400</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D203">
+        <v>24800400</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>25020004</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D204">
+        <v>25020004</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>25200400</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D205">
+        <v>25200400</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>25361296</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D206">
+        <v>25361296</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>25593481</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D207">
+        <v>25593481</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>25715041</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D208">
+        <v>25715041</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>26020201</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D209">
+        <v>26020201</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>26030404</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D210">
+        <v>26030404</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>26553409</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D211">
+        <v>26553409</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>26563716</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D212">
+        <v>26563716</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>26604964</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D213">
+        <v>26604964</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>26635921</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D214">
+        <v>26635921</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>26759929</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D215">
+        <v>26759929</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>27060804</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D216">
+        <v>27060804</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>27520516</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D217">
+        <v>27520516</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>27531009</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D218">
+        <v>27531009</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>27594009</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D219">
+        <v>27594009</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>27615025</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D220">
+        <v>27615025</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>27899524</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D221">
+        <v>27899524</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>27952369</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D222">
+        <v>27952369</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>28026436</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D223">
+        <v>28026436</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>28334329</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D224">
+        <v>28334329</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>28451556</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D225">
+        <v>28451556</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>29127609</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D226">
+        <v>29127609</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>29235649</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D227">
+        <v>29235649</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>29571844</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D228">
+        <v>29571844</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>29637136</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D229">
+        <v>29637136</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>30008484</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D230">
+        <v>30008484</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>30217009</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D231">
+        <v>30217009</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>30316036</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D232">
+        <v>30316036</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>30713764</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D233">
+        <v>30713764</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>31158724</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D234">
+        <v>31158724</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>31304025</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D235">
+        <v>31304025</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>31629376</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D236">
+        <v>31629376</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>32171584</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D237">
+        <v>32171584</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>32307856</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D238">
+        <v>32307856</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>32752729</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D239">
+        <v>32752729</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>33396841</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D240">
+        <v>33396841</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>33524100</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D241">
+        <v>33524100</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>33732864</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D242">
+        <v>33732864</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>34774609</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D243">
+        <v>34774609</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>35034561</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D244">
+        <v>35034561</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>35058241</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D245">
+        <v>35058241</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>35295481</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D246">
+        <v>35295481</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>35521600</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D247">
+        <v>35521600</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>35628961</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D248">
+        <v>35628961</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>35676729</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D249">
+        <v>35676729</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>35748441</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D250">
+        <v>35748441</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>36024004</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D251">
+        <v>36024004</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>36156169</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D252">
+        <v>36156169</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>36192256</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D253">
+        <v>36192256</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>36240400</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D254">
+        <v>36240400</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>36372961</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D255">
+        <v>36372961</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>36505764</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D256">
+        <v>36505764</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>36820624</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D257">
+        <v>36820624</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>37027225</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D258">
+        <v>37027225</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>37332100</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D259">
+        <v>37332100</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>38056561</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D260">
+        <v>38056561</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>38551681</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D261">
+        <v>38551681</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>39200121</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D262">
+        <v>39200121</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>39463524</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D263">
+        <v>39463524</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>39639616</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D264">
+        <v>39639616</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>39891856</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D265">
+        <v>39891856</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>40335201</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D266">
+        <v>40335201</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>41242084</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D267">
+        <v>41242084</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>41434969</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D268">
+        <v>41434969</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>41499364</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D269">
+        <v>41499364</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>41538025</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D270">
+        <v>41538025</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>42250000</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D271">
+        <v>42250000</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>43256929</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D272">
+        <v>43256929</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>43414921</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D273">
+        <v>43414921</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>43718544</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D274">
+        <v>43718544</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>43758225</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D275">
+        <v>43758225</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>44169316</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D276">
+        <v>44169316</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>44275716</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D277">
+        <v>44275716</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>44395569</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D278">
+        <v>44395569</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>45792289</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D279">
+        <v>45792289</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>45914176</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D280">
+        <v>45914176</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>46335249</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D281">
+        <v>46335249</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>46703556</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D282">
+        <v>46703556</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>46826649</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D283">
+        <v>46826649</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>47141956</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D284">
+        <v>47141956</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>47430769</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D285">
+        <v>47430769</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>48525156</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D286">
+        <v>48525156</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>48888064</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D287">
+        <v>48888064</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>49350625</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D288">
+        <v>49350625</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>49434961</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D289">
+        <v>49434961</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>49857721</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D290">
+        <v>49857721</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>50495236</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D291">
+        <v>50495236</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>50637456</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D292">
+        <v>50637456</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>50879689</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D293">
+        <v>50879689</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>51051025</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D294">
+        <v>51051025</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>51652969</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D295">
+        <v>51652969</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>51782416</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D296">
+        <v>51782416</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>52215076</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D297">
+        <v>52215076</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>53085796</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D298">
+        <v>53085796</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>53158681</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D299">
+        <v>53158681</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>53231616</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D300">
+        <v>53231616</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>53494596</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D301">
+        <v>53494596</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>53714241</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D302">
+        <v>53714241</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>53758224</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D303">
+        <v>53758224</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>54390625</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D304">
+        <v>54390625</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>54479161</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D305">
+        <v>54479161</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>55071241</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D306">
+        <v>55071241</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>55547209</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D307">
+        <v>55547209</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>55771024</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D308">
+        <v>55771024</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>55845729</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D309">
+        <v>55845729</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>56235001</v>
       </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D310">
+        <v>56235001</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>57229225</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D311">
+        <v>57229225</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>58155876</v>
       </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D312">
+        <v>58155876</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>58232161</v>
       </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D313">
+        <v>58232161</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>58614336</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D314">
+        <v>58614336</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>58813561</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D315">
+        <v>58813561</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>59043856</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D316">
+        <v>59043856</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>59521225</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D317">
+        <v>59521225</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>60233121</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D318">
+        <v>60233121</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>60637369</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D319">
+        <v>60637369</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>60777616</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D320">
+        <v>60777616</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>61121124</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D321">
+        <v>61121124</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>61136761</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D322">
+        <v>61136761</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>62031376</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D323">
+        <v>62031376</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>62837329</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D324">
+        <v>62837329</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>63313849</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D325">
+        <v>63313849</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>63345681</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D326">
+        <v>63345681</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>63536841</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D327">
+        <v>63536841</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>64032004</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D328">
+        <v>64032004</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>64176121</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D329">
+        <v>64176121</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>64320400</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D330">
+        <v>64320400</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>64899136</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D331">
+        <v>64899136</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>65237929</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D332">
+        <v>65237929</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>65755881</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D333">
+        <v>65755881</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>66113161</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D334">
+        <v>66113161</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>66373609</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D335">
+        <v>66373609</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>66422500</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D336">
+        <v>66422500</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>66732561</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D337">
+        <v>66732561</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>69655716</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D338">
+        <v>69655716</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>69705801</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D339">
+        <v>69705801</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>69973225</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D340">
+        <v>69973225</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>70392100</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D341">
+        <v>70392100</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>70711281</v>
       </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D342">
+        <v>70711281</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>70997476</v>
       </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D343">
+        <v>70997476</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>71740900</v>
       </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D344">
+        <v>71740900</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>72029169</v>
       </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D345">
+        <v>72029169</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>72165025</v>
       </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D346">
+        <v>72165025</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>72301009</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D347">
+        <v>72301009</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>73034116</v>
       </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D348">
+        <v>73034116</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>73051209</v>
       </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D349">
+        <v>73051209</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>73136704</v>
       </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D350">
+        <v>73136704</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>73702225</v>
       </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D351">
+        <v>73702225</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>74425129</v>
       </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D352">
+        <v>74425129</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>74787904</v>
       </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D353">
+        <v>74787904</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>74909025</v>
       </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D354">
+        <v>74909025</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>75168900</v>
       </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D355">
+        <v>75168900</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>75186241</v>
       </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D356">
+        <v>75186241</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>75481344</v>
       </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D357">
+        <v>75481344</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>75498721</v>
       </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D358">
+        <v>75498721</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>75986089</v>
       </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D359">
+        <v>75986089</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>76143076</v>
       </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D360">
+        <v>76143076</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>76195441</v>
       </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D361">
+        <v>76195441</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>76230361</v>
       </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D362">
+        <v>76230361</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>76632516</v>
       </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D363">
+        <v>76632516</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>76983076</v>
       </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D364">
+        <v>76983076</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>77457601</v>
       </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D365">
+        <v>77457601</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>77704225</v>
       </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D366">
+        <v>77704225</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>78039556</v>
       </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D367">
+        <v>78039556</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>78712384</v>
       </c>
-    </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D368">
+        <v>78712384</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>79032100</v>
       </c>
-    </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D369">
+        <v>79032100</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>79584241</v>
       </c>
-    </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D370">
+        <v>79584241</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>80048809</v>
       </c>
-    </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D371">
+        <v>80048809</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>80281600</v>
       </c>
-    </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D372">
+        <v>80281600</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>81631225</v>
       </c>
-    </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D373">
+        <v>81631225</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>81757764</v>
       </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D374">
+        <v>81757764</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>82228624</v>
       </c>
-    </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D375">
+        <v>82228624</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>82591744</v>
       </c>
-    </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D376">
+        <v>82591744</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>82646281</v>
       </c>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D377">
+        <v>82646281</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>84088900</v>
       </c>
-    </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D378">
+        <v>84088900</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>84879369</v>
       </c>
-    </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D379">
+        <v>84879369</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>84971524</v>
       </c>
-    </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D380">
+        <v>84971524</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>85008400</v>
       </c>
-    </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D381">
+        <v>85008400</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>85192900</v>
       </c>
-    </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D382">
+        <v>85192900</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>85877289</v>
       </c>
-    </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D383">
+        <v>85877289</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>86155524</v>
       </c>
-    </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D384">
+        <v>86155524</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>86266944</v>
       </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D385">
+        <v>86266944</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>86452804</v>
       </c>
-    </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D386">
+        <v>86452804</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>86806489</v>
       </c>
-    </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D387">
+        <v>86806489</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>87815641</v>
       </c>
-    </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D388">
+        <v>87815641</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>88717561</v>
       </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D389">
+        <v>88717561</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>89889361</v>
       </c>
-    </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D390">
+        <v>89889361</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>91661476</v>
       </c>
-    </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D391">
+        <v>91661476</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>92217609</v>
       </c>
-    </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D392">
+        <v>92217609</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>93412225</v>
       </c>
-    </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D393">
+        <v>93412225</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>93818596</v>
       </c>
-    </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D394">
+        <v>93818596</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>94109401</v>
       </c>
-    </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D395">
+        <v>94109401</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>94167616</v>
       </c>
-    </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D396">
+        <v>94167616</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>94497841</v>
       </c>
-    </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D397">
+        <v>94497841</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>94517284</v>
       </c>
-    </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D398">
+        <v>94517284</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>94945536</v>
       </c>
-    </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D399">
+        <v>94945536</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>95394289</v>
       </c>
-    </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D400">
+        <v>95394289</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>95922436</v>
       </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D401">
+        <v>95922436</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>96255721</v>
       </c>
-    </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D402">
+        <v>96255721</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>96550276</v>
       </c>
-    </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D403">
+        <v>96550276</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>97772544</v>
       </c>
-    </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D404">
+        <v>97772544</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>98109025</v>
       </c>
-    </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D405">
+        <v>98109025</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>99102025</v>
       </c>
-    </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D406">
+        <v>99102025</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D407">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>100881936</v>
       </c>
-    </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D408">
+        <v>100881936</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>101425041</v>
       </c>
-    </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D409">
+        <v>101425041</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>102171664</v>
       </c>
-    </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D410">
+        <v>102171664</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>102232321</v>
       </c>
-    </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D411">
+        <v>102232321</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>102515625</v>
       </c>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D412">
+        <v>102515625</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>103164649</v>
       </c>
-    </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D413">
+        <v>103164649</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>103286569</v>
       </c>
-    </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D414">
+        <v>103286569</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>103449241</v>
       </c>
-    </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D415">
+        <v>103449241</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>105083001</v>
       </c>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D416">
+        <v>105083001</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>105144516</v>
       </c>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D417">
+        <v>105144516</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>106172416</v>
       </c>
-    </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D418">
+        <v>106172416</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>106275481</v>
       </c>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D419">
+        <v>106275481</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>107143201</v>
       </c>
-    </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D420">
+        <v>107143201</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>107785924</v>
       </c>
-    </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D421">
+        <v>107785924</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>108826624</v>
       </c>
-    </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D422">
+        <v>108826624</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>109098025</v>
       </c>
-    </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D423">
+        <v>109098025</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>109307025</v>
       </c>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D424">
+        <v>109307025</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>109474369</v>
       </c>
-    </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D425">
+        <v>109474369</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>109725625</v>
       </c>
-    </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D426">
+        <v>109725625</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>110502144</v>
       </c>
-    </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D427">
+        <v>110502144</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>110565225</v>
       </c>
-    </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D428">
+        <v>110565225</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>110796676</v>
       </c>
-    </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D429">
+        <v>110796676</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>111091600</v>
       </c>
-    </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D430">
+        <v>111091600</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>111746041</v>
       </c>
-    </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D431">
+        <v>111746041</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>113678244</v>
       </c>
-    </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D432">
+        <v>113678244</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>114169225</v>
       </c>
-    </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D433">
+        <v>114169225</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>114233344</v>
       </c>
-    </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D434">
+        <v>114233344</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>114340249</v>
       </c>
-    </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D435">
+        <v>114340249</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>114554209</v>
       </c>
-    </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D436">
+        <v>114554209</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>115025625</v>
       </c>
-    </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D437">
+        <v>115025625</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>115863696</v>
       </c>
-    </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D438">
+        <v>115863696</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>115949824</v>
       </c>
-    </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D439">
+        <v>115949824</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>116445681</v>
       </c>
-    </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D440">
+        <v>116445681</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>116748025</v>
       </c>
-    </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D441">
+        <v>116748025</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>117440569</v>
       </c>
-    </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D442">
+        <v>117440569</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>117548964</v>
       </c>
-    </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D443">
+        <v>117548964</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>118265625</v>
       </c>
-    </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D444">
+        <v>118265625</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>118461456</v>
       </c>
-    </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D445">
+        <v>118461456</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>118657449</v>
       </c>
-    </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D446">
+        <v>118657449</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>119224561</v>
       </c>
-    </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D447">
+        <v>119224561</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>120582361</v>
       </c>
-    </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D448">
+        <v>120582361</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>121176064</v>
       </c>
-    </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D449">
+        <v>121176064</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>121242121</v>
       </c>
-    </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D450">
+        <v>121242121</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>121550625</v>
       </c>
-    </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D451">
+        <v>121550625</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>121638841</v>
       </c>
-    </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D452">
+        <v>121638841</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>121705024</v>
       </c>
-    </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D453">
+        <v>121705024</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>122014116</v>
       </c>
-    </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D454">
+        <v>122014116</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A455">
         <v>122301481</v>
       </c>
-    </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D455">
+        <v>122301481</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A456">
         <v>122389969</v>
       </c>
-    </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D456">
+        <v>122389969</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A457">
         <v>122899396</v>
       </c>
-    </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D457">
+        <v>122899396</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A458">
         <v>122943744</v>
       </c>
-    </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D458">
+        <v>122943744</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>123232201</v>
       </c>
-    </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D459">
+        <v>123232201</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A460">
         <v>123988225</v>
       </c>
-    </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D460">
+        <v>123988225</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A461">
         <v>124925329</v>
       </c>
-    </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D461">
+        <v>124925329</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A462">
         <v>125686521</v>
       </c>
-    </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D462">
+        <v>125686521</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463">
         <v>125708944</v>
       </c>
-    </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D463">
+        <v>125708944</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A464">
         <v>126337600</v>
       </c>
-    </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D464">
+        <v>126337600</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A465">
         <v>127035441</v>
       </c>
-    </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D465">
+        <v>127035441</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A466">
         <v>127057984</v>
       </c>
-    </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D466">
+        <v>127057984</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A467">
         <v>127893481</v>
       </c>
-    </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D467">
+        <v>127893481</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A468">
         <v>128323584</v>
       </c>
-    </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D468">
+        <v>128323584</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A469">
         <v>128527569</v>
       </c>
-    </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D469">
+        <v>128527569</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A470">
         <v>128754409</v>
       </c>
-    </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D470">
+        <v>128754409</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A471">
         <v>129254161</v>
       </c>
-    </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D471">
+        <v>129254161</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A472">
         <v>129276900</v>
       </c>
-    </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D472">
+        <v>129276900</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A473">
         <v>132089049</v>
       </c>
-    </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D473">
+        <v>132089049</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A474">
         <v>132388036</v>
       </c>
-    </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D474">
+        <v>132388036</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A475">
         <v>132457081</v>
       </c>
-    </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D475">
+        <v>132457081</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A476">
         <v>133402500</v>
       </c>
-    </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D476">
+        <v>133402500</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A477">
         <v>133726096</v>
       </c>
-    </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D477">
+        <v>133726096</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A478">
         <v>134003776</v>
       </c>
-    </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D478">
+        <v>134003776</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A479">
         <v>134722449</v>
       </c>
-    </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D479">
+        <v>134722449</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A480">
         <v>136188900</v>
       </c>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D480">
+        <v>136188900</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A481">
         <v>136328976</v>
       </c>
-    </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D481">
+        <v>136328976</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A482">
         <v>136656100</v>
       </c>
-    </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D482">
+        <v>136656100</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A483">
         <v>137124100</v>
       </c>
-    </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D483">
+        <v>137124100</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A484">
         <v>137663289</v>
       </c>
-    </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D484">
+        <v>137663289</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A485">
         <v>141348321</v>
       </c>
-    </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D485">
+        <v>141348321</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A486">
         <v>141372100</v>
       </c>
-    </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D486">
+        <v>141372100</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A487">
         <v>142348761</v>
       </c>
-    </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D487">
+        <v>142348761</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A488">
         <v>143209089</v>
       </c>
-    </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D488">
+        <v>143209089</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A489">
         <v>143856036</v>
       </c>
-    </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D489">
+        <v>143856036</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A490">
         <v>143928009</v>
       </c>
-    </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D490">
+        <v>143928009</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A491">
         <v>145274809</v>
       </c>
-    </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D491">
+        <v>145274809</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A492">
         <v>145805625</v>
       </c>
-    </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D492">
+        <v>145805625</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A493">
         <v>147501025</v>
       </c>
-    </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D493">
+        <v>147501025</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A494">
         <v>147671104</v>
       </c>
-    </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D494">
+        <v>147671104</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>147889921</v>
       </c>
-    </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D495">
+        <v>147889921</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>148011556</v>
       </c>
-    </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D496">
+        <v>148011556</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>148035889</v>
       </c>
-    </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D497">
+        <v>148035889</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>148133241</v>
       </c>
-    </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D498">
+        <v>148133241</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>149132944</v>
       </c>
-    </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D499">
+        <v>149132944</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>149377284</v>
       </c>
-    </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D500">
+        <v>149377284</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A501">
+        <v>150038001</v>
+      </c>
+      <c r="D501">
         <v>150038001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I figured out why the squared input makes sense. Now why increment by 4?
</commit_message>
<xml_diff>
--- a/Excel_Challenge_508 - Number is Perfect Square and Sum of Squares of Digits is also a Perfect Square.xlsx
+++ b/Excel_Challenge_508 - Number is Perfect Square and Sum of Squares of Digits is also a Perfect Square.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AD438E-F2BC-48D9-AD3C-DE87C95EA86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B850F1-C0C0-47E9-9A3B-3003F6E75D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,12 +59,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Answer Expected</t>
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7222450587827601408/</t>
+  </si>
+  <si>
+    <t>Using a squared sequence makes sense because we only should be looking at perfect squares.</t>
+  </si>
+  <si>
+    <t>Why increment by 4?</t>
   </si>
 </sst>
 </file>
@@ -3116,8 +3122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34D53AD-D1D9-449B-ADBF-99E3A90ED89B}">
   <dimension ref="A1:K501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A496" workbookViewId="0">
-      <selection activeCell="H498" sqref="H498"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3149,6 +3155,9 @@
 _xlfn.DROP(_xlpm.z,1))</f>
         <v>100</v>
       </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -3156,6 +3165,9 @@
       </c>
       <c r="D3">
         <v>400</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>